<commit_message>
Getting all target tests workign
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baroa\eclipse-workspace\ClueGame\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cades\OneDrive\Desktop\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E64EBB-085B-417C-9331-AA0A6677D65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17417566-6DAA-4E79-A8FE-624A519348C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{57D85AC3-8786-4516-A829-142AFE2E1374}"/>
+    <workbookView xWindow="8378" yWindow="0" windowWidth="8625" windowHeight="10643" xr2:uid="{57D85AC3-8786-4516-A829-142AFE2E1374}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="38">
   <si>
     <t>W</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>W^</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>testing targets</t>
+  </si>
+  <si>
+    <t>testing adjacency</t>
   </si>
 </sst>
 </file>
@@ -156,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +256,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -276,6 +297,8 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,15 +633,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8704207-248F-460E-B715-D5924E5B563A}">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -692,7 +715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -711,7 +734,7 @@
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -769,7 +792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -846,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -913,7 +936,7 @@
       <c r="V4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="W4" s="16" t="s">
         <v>18</v>
       </c>
       <c r="X4" s="6" t="s">
@@ -922,8 +945,15 @@
       <c r="Y4" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="AA4" s="15"/>
+      <c r="AB4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+1</f>
         <v>3</v>
@@ -946,7 +976,7 @@
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -1000,8 +1030,15 @@
       <c r="Y5" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="AA5" s="16"/>
+      <c r="AB5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A26" si="0">A5+1</f>
         <v>4</v>
@@ -1015,7 +1052,7 @@
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1079,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1109,7 +1146,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>3</v>
@@ -1130,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>3</v>
@@ -1157,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1235,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1285,7 +1322,7 @@
       <c r="P9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -1313,7 +1350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1327,7 +1364,7 @@
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1351,7 +1388,7 @@
       <c r="L10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="16" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -1375,7 +1412,7 @@
       <c r="T10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="14" t="s">
+      <c r="U10" s="16" t="s">
         <v>33</v>
       </c>
       <c r="V10" s="10" t="s">
@@ -1391,7 +1428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1417,7 +1454,7 @@
       <c r="H11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="15" t="s">
         <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1459,7 +1496,7 @@
       <c r="V11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="W11" s="15" t="s">
         <v>30</v>
       </c>
       <c r="X11" s="10" t="s">
@@ -1469,7 +1506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1547,7 +1584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1621,11 +1658,11 @@
       <c r="X13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Y13" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1636,7 +1673,7 @@
       <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -1703,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1729,7 +1766,7 @@
       <c r="H15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="15" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -1781,7 +1818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1885,7 +1922,7 @@
       <c r="H17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="15" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -1903,7 +1940,7 @@
       <c r="N17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="16" t="s">
         <v>0</v>
       </c>
       <c r="P17" s="1" t="s">
@@ -1927,7 +1964,7 @@
       <c r="V17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="W17" s="13" t="s">
+      <c r="W17" s="16" t="s">
         <v>28</v>
       </c>
       <c r="X17" s="11" t="s">
@@ -2065,7 +2102,7 @@
       <c r="P19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="16" t="s">
         <v>31</v>
       </c>
       <c r="R19" s="1" t="s">
@@ -2344,7 +2381,7 @@
       <c r="E23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2365,7 +2402,7 @@
       <c r="L23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="M23" s="16" t="s">
         <v>24</v>
       </c>
       <c r="N23" s="8" t="s">
@@ -2491,7 +2528,7 @@
       <c r="B25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7" t="s">

</xml_diff>